<commit_message>
update prototype_5a, this closes #3
</commit_message>
<xml_diff>
--- a/planning/5a_prototype.xlsx
+++ b/planning/5a_prototype.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20225"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="23426"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://tecmx-my.sharepoint.com/personal/a01730565_itesm_mx/Documents/Desktop/ITESM/7mo/IIS/5a/planning/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="2" documentId="11_56D7563A6D94B9B9A15889D9AC9BE360D5050994" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{EAF896A0-58A2-40C0-A618-70AF55375A03}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25520" windowHeight="15600" tabRatio="500" activeTab="3"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" tabRatio="500" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="triangulo" sheetId="1" r:id="rId1"/>
@@ -12,8 +18,17 @@
     <sheet name="1 entre x" sheetId="5" r:id="rId3"/>
     <sheet name="t-student" sheetId="4" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="140001" concurrentCalc="0"/>
+  <calcPr calcId="191029" concurrentCalc="0"/>
   <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
     </ext>
@@ -162,7 +177,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0000000000"/>
   </numFmts>
@@ -318,11 +333,19 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="es-ES"/>
   <c:roundedCorners val="0"/>
@@ -354,19 +377,19 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>0.0</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1.0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>2.0</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>3.0</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>4.0</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -378,24 +401,29 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>0.0</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2.0</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>4.0</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>6.0</c:v>
+                  <c:v>6</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>8.0</c:v>
+                  <c:v>8</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:yVal>
           <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-EF3C-4FB2-B421-B5CFD47485A0}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:dLbls>
           <c:showLegendKey val="0"/>
@@ -450,14 +478,14 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="1.0" l="0.75" r="0.75" t="1.0" header="0.5" footer="0.5"/>
+    <c:pageMargins b="1" l="0.75" r="0.75" t="1" header="0.5" footer="0.5"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
 </file>
 
 <file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="es-ES"/>
   <c:roundedCorners val="0"/>
@@ -489,7 +517,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>0.0</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>0.25</c:v>
@@ -501,7 +529,7 @@
                   <c:v>0.75</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1.0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -513,10 +541,10 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>0.0</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.0625</c:v>
+                  <c:v>6.25E-2</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>0.25</c:v>
@@ -525,12 +553,17 @@
                   <c:v>0.5625</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1.0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:yVal>
           <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-023D-4682-A017-B8F287ACA319}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:dLbls>
           <c:showLegendKey val="0"/>
@@ -577,7 +610,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -586,14 +618,14 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="1.0" l="0.75" r="0.75" t="1.0" header="0.5" footer="0.5"/>
+    <c:pageMargins b="1" l="0.75" r="0.75" t="1" header="0.5" footer="0.5"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
 </file>
 
 <file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="es-ES"/>
   <c:roundedCorners val="0"/>
@@ -625,25 +657,25 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>1.0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>1.5</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>2.0</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>2.5</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>3.0</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>3.5</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>4.0</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -655,10 +687,10 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>1.0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.666666666666667</c:v>
+                  <c:v>0.66666666666666663</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>0.5</c:v>
@@ -667,10 +699,10 @@
                   <c:v>0.4</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.333333333333333</c:v>
+                  <c:v>0.33333333333333331</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.285714285714286</c:v>
+                  <c:v>0.2857142857142857</c:v>
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>0.25</c:v>
@@ -679,6 +711,11 @@
             </c:numRef>
           </c:yVal>
           <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-CB89-47E8-8BD7-1783729242A2}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:dLbls>
           <c:showLegendKey val="0"/>
@@ -725,7 +762,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -734,14 +770,14 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="1.0" l="0.75" r="0.75" t="1.0" header="0.5" footer="0.5"/>
+    <c:pageMargins b="1" l="0.75" r="0.75" t="1" header="0.5" footer="0.5"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
 </file>
 
 <file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="es-ES"/>
   <c:roundedCorners val="0"/>
@@ -773,7 +809,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="13"/>
                 <c:pt idx="0">
-                  <c:v>1.0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>1.25</c:v>
@@ -785,7 +821,7 @@
                   <c:v>1.75</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>2.0</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>2.25</c:v>
@@ -797,7 +833,7 @@
                   <c:v>2.75</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>3.0</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="9">
                   <c:v>3.25</c:v>
@@ -809,7 +845,7 @@
                   <c:v>3.75</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>4.0</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -821,40 +857,40 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="13"/>
                 <c:pt idx="0">
-                  <c:v>1.0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>0.8</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.666666666666667</c:v>
+                  <c:v>0.66666666666666663</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.571428571428571</c:v>
+                  <c:v>0.5714285714285714</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>0.5</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.444444444444444</c:v>
+                  <c:v>0.44444444444444442</c:v>
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>0.4</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.363636363636364</c:v>
+                  <c:v>0.36363636363636365</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.333333333333333</c:v>
+                  <c:v>0.33333333333333331</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0.307692307692308</c:v>
+                  <c:v>0.30769230769230771</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0.285714285714286</c:v>
+                  <c:v>0.2857142857142857</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>0.266666666666667</c:v>
+                  <c:v>0.26666666666666666</c:v>
                 </c:pt>
                 <c:pt idx="12">
                   <c:v>0.25</c:v>
@@ -863,6 +899,11 @@
             </c:numRef>
           </c:yVal>
           <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-1ED6-43B0-9F59-DFE73FA3F41D}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:dLbls>
           <c:showLegendKey val="0"/>
@@ -909,7 +950,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -918,14 +958,14 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="1.0" l="0.75" r="0.75" t="1.0" header="0.5" footer="0.5"/>
+    <c:pageMargins b="1" l="0.75" r="0.75" t="1" header="0.5" footer="0.5"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
 </file>
 
 <file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="es-ES"/>
   <c:roundedCorners val="0"/>
@@ -957,22 +997,22 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="11"/>
                 <c:pt idx="0">
-                  <c:v>0.0</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.11</c:v>
+                  <c:v>0.11000000000000001</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.22</c:v>
+                  <c:v>0.22000000000000003</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.33</c:v>
+                  <c:v>0.33000000000000007</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.44</c:v>
+                  <c:v>0.44000000000000006</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.55</c:v>
+                  <c:v>0.55000000000000004</c:v>
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>0.66</c:v>
@@ -987,7 +1027,7 @@
                   <c:v>0.99</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>1.1</c:v>
+                  <c:v>1.1000000000000001</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -999,42 +1039,47 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="11"/>
                 <c:pt idx="0">
-                  <c:v>0.388034908871669</c:v>
+                  <c:v>0.38803490887166864</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.385436939844832</c:v>
+                  <c:v>0.38543693984483202</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.377767323980263</c:v>
+                  <c:v>0.37776732398026314</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.365387489607798</c:v>
+                  <c:v>0.36538748960779854</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.348863331270197</c:v>
+                  <c:v>0.34886333127019753</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.328915963281718</c:v>
+                  <c:v>0.32891596328171852</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.306362592894306</c:v>
+                  <c:v>0.30636259289430617</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.282054971406634</c:v>
+                  <c:v>0.28205497140663432</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.256822344419287</c:v>
+                  <c:v>0.25682234441928659</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0.231424258297114</c:v>
+                  <c:v>0.23142425829711369</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0.206516442244851</c:v>
+                  <c:v>0.20651644224485097</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:yVal>
           <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-1C7C-4D51-B4AD-092E23E2EF64}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:dLbls>
           <c:showLegendKey val="0"/>
@@ -1081,7 +1126,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -1090,14 +1134,14 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="1.0" l="0.75" r="0.75" t="1.0" header="0.5" footer="0.5"/>
+    <c:pageMargins b="1" l="0.75" r="0.75" t="1" header="0.5" footer="0.5"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
 </file>
 
 <file path=xl/charts/chart6.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="es-ES"/>
   <c:roundedCorners val="0"/>
@@ -1129,28 +1173,28 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="21"/>
                 <c:pt idx="0">
-                  <c:v>0.0</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.055</c:v>
+                  <c:v>5.5000000000000007E-2</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.11</c:v>
+                  <c:v>0.11000000000000001</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.165</c:v>
+                  <c:v>0.16500000000000004</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.22</c:v>
+                  <c:v>0.22000000000000003</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.275</c:v>
+                  <c:v>0.27500000000000002</c:v>
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>0.33</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.385</c:v>
+                  <c:v>0.38500000000000001</c:v>
                 </c:pt>
                 <c:pt idx="8">
                   <c:v>0.44</c:v>
@@ -1159,37 +1203,37 @@
                   <c:v>0.495</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0.55</c:v>
+                  <c:v>0.55000000000000004</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>0.605</c:v>
+                  <c:v>0.60500000000000009</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>0.66</c:v>
+                  <c:v>0.66000000000000014</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>0.715</c:v>
+                  <c:v>0.71500000000000019</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>0.77</c:v>
+                  <c:v>0.77000000000000024</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>0.825</c:v>
+                  <c:v>0.82500000000000029</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>0.88</c:v>
+                  <c:v>0.88000000000000034</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>0.935</c:v>
+                  <c:v>0.93500000000000039</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>0.99</c:v>
+                  <c:v>0.99000000000000044</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>1.045</c:v>
+                  <c:v>1.0450000000000004</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>1.1</c:v>
+                  <c:v>1.1000000000000003</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1201,72 +1245,77 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="21"/>
                 <c:pt idx="0">
-                  <c:v>0.393729807292604</c:v>
+                  <c:v>0.39372980729260415</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.393103496559054</c:v>
+                  <c:v>0.39310349655905424</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.391231130401122</c:v>
+                  <c:v>0.39123113040112251</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.388132282008527</c:v>
+                  <c:v>0.38813228200852751</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.383839160500853</c:v>
+                  <c:v>0.38383916050085343</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.378396004083139</c:v>
+                  <c:v>0.37839600408313939</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.371858254856815</c:v>
+                  <c:v>0.3718582548568149</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.364291538520867</c:v>
+                  <c:v>0.3642915385208671</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.355770477249064</c:v>
+                  <c:v>0.35577047724906408</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0.346377368002137</c:v>
+                  <c:v>0.34637736800213692</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0.33620076130558</c:v>
+                  <c:v>0.33620076130558002</c:v>
                 </c:pt>
                 <c:pt idx="11">
                   <c:v>0.325333977028884</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>0.313873593934048</c:v>
+                  <c:v>0.31387359393404801</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>0.30191794877051</c:v>
+                  <c:v>0.30191794877051004</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>0.289565678581538</c:v>
+                  <c:v>0.28956567858153792</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>0.27691433679853</c:v>
+                  <c:v>0.27691433679853023</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>0.264059109812576</c:v>
+                  <c:v>0.26405910981257602</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>0.2510916562275</c:v>
+                  <c:v>0.25109165622749963</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>0.238099086126603</c:v>
+                  <c:v>0.23809908612660322</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>0.2251630926374</c:v>
+                  <c:v>0.22516309263740014</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>0.212359243055184</c:v>
+                  <c:v>0.21235924305518386</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:yVal>
           <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-8EF0-4FB1-A29C-B2C3D061B059}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:dLbls>
           <c:showLegendKey val="0"/>
@@ -1313,7 +1362,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -1322,7 +1370,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="1.0" l="0.75" r="0.75" t="1.0" header="0.5" footer="0.5"/>
+    <c:pageMargins b="1" l="0.75" r="0.75" t="1" header="0.5" footer="0.5"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -1345,7 +1393,13 @@
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="4" name="Gráfico 3"/>
+        <xdr:cNvPr id="4" name="Gráfico 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000004000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -1375,7 +1429,13 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="3" name="Imagen 2" descr="simpson_rule.png"/>
+        <xdr:cNvPr id="3" name="Imagen 2" descr="simpson_rule.png">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000003000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -1424,7 +1484,13 @@
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="2" name="Gráfico 1"/>
+        <xdr:cNvPr id="2" name="Gráfico 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000002000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvGraphicFramePr>
           <a:graphicFrameLocks/>
         </xdr:cNvGraphicFramePr>
@@ -1456,7 +1522,13 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="3" name="Imagen 2" descr="simpson_rule.png"/>
+        <xdr:cNvPr id="3" name="Imagen 2" descr="simpson_rule.png">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000003000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -1505,7 +1577,13 @@
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="2" name="Gráfico 1"/>
+        <xdr:cNvPr id="2" name="Gráfico 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000002000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvGraphicFramePr>
           <a:graphicFrameLocks/>
         </xdr:cNvGraphicFramePr>
@@ -1537,7 +1615,13 @@
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="3" name="Gráfico 2"/>
+        <xdr:cNvPr id="3" name="Gráfico 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000003000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -1572,7 +1656,13 @@
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="2" name="Gráfico 1"/>
+        <xdr:cNvPr id="2" name="Gráfico 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-000002000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvGraphicFramePr>
           <a:graphicFrameLocks/>
         </xdr:cNvGraphicFramePr>
@@ -1604,7 +1694,13 @@
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="3" name="Gráfico 2"/>
+        <xdr:cNvPr id="3" name="Gráfico 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-000003000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -1621,20 +1717,26 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>651937</xdr:colOff>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
       <xdr:row>22</xdr:row>
-      <xdr:rowOff>64986</xdr:rowOff>
+      <xdr:rowOff>628</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>914403</xdr:colOff>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>1197061</xdr:colOff>
       <xdr:row>26</xdr:row>
-      <xdr:rowOff>194732</xdr:rowOff>
+      <xdr:rowOff>130374</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="4" name="Imagen 3" descr="distribucionT.png"/>
+        <xdr:cNvPr id="4" name="Imagen 3" descr="distribucionT.png">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-000004000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -1653,8 +1755,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="2184404" y="4349119"/>
-          <a:ext cx="7078132" cy="908680"/>
+          <a:off x="0" y="4531439"/>
+          <a:ext cx="5624899" cy="953530"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1987,19 +2089,19 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G21"/>
   <sheetViews>
     <sheetView zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
       <selection activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="9.1640625" customWidth="1"/>
+    <col min="2" max="2" width="9.125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>26</v>
       </c>
@@ -2010,7 +2112,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:6">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>27</v>
       </c>
@@ -2021,7 +2123,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:6">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B3" s="2" t="s">
         <v>1</v>
       </c>
@@ -2029,7 +2131,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:6">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>29</v>
       </c>
@@ -2048,7 +2150,7 @@
         <v>0.33333333333333331</v>
       </c>
     </row>
-    <row r="7" spans="1:6">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B7" s="6" t="s">
         <v>0</v>
       </c>
@@ -2056,7 +2158,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="8" spans="1:6">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B8" s="6"/>
       <c r="C8" s="6"/>
       <c r="D8" t="s">
@@ -2066,7 +2168,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="9" spans="1:6">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B9" s="6">
         <v>0</v>
       </c>
@@ -2086,7 +2188,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:6">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B10" s="6">
         <f>B9+$C$5</f>
         <v>1</v>
@@ -2107,7 +2209,7 @@
         <v>2.6666666666666665</v>
       </c>
     </row>
-    <row r="11" spans="1:6">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B11" s="6">
         <f t="shared" ref="B11:B13" si="3">B10+$C$5</f>
         <v>2</v>
@@ -2128,7 +2230,7 @@
         <v>2.6666666666666665</v>
       </c>
     </row>
-    <row r="12" spans="1:6">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B12" s="6">
         <f t="shared" si="3"/>
         <v>3</v>
@@ -2149,7 +2251,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="13" spans="1:6">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B13" s="6">
         <f t="shared" si="3"/>
         <v>4</v>
@@ -2170,12 +2272,12 @@
         <v>2.6666666666666665</v>
       </c>
     </row>
-    <row r="14" spans="1:6">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C14" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="15" spans="1:6">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D15" t="s">
         <v>4</v>
       </c>
@@ -2188,7 +2290,7 @@
         <v>15.999999999999998</v>
       </c>
     </row>
-    <row r="16" spans="1:6">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D16" t="s">
         <v>5</v>
       </c>
@@ -2199,7 +2301,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="17" spans="3:7">
+    <row r="17" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C17" t="s">
         <v>35</v>
       </c>
@@ -2216,7 +2318,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="18" spans="3:7">
+    <row r="18" spans="3:7" x14ac:dyDescent="0.25">
       <c r="F18">
         <v>0</v>
       </c>
@@ -2224,18 +2326,18 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="3:7">
+    <row r="19" spans="3:7" x14ac:dyDescent="0.25">
       <c r="F19" s="7">
         <f>F17-F18</f>
         <v>16</v>
       </c>
     </row>
-    <row r="20" spans="3:7">
+    <row r="20" spans="3:7" x14ac:dyDescent="0.25">
       <c r="F20" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="21" spans="3:7">
+    <row r="21" spans="3:7" x14ac:dyDescent="0.25">
       <c r="F21" t="s">
         <v>5</v>
       </c>
@@ -2252,20 +2354,20 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:F21"/>
   <sheetViews>
     <sheetView zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
       <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="9.1640625" customWidth="1"/>
+    <col min="2" max="2" width="9.125" customWidth="1"/>
     <col min="5" max="5" width="17.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>37</v>
       </c>
@@ -2276,7 +2378,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:6">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>38</v>
       </c>
@@ -2287,7 +2389,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:6">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B3" s="1" t="s">
         <v>1</v>
       </c>
@@ -2295,7 +2397,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:6">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
         <v>2</v>
       </c>
@@ -2311,7 +2413,7 @@
         <v>8.3333333333333329E-2</v>
       </c>
     </row>
-    <row r="6" spans="1:6">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="E6" t="s">
         <v>5</v>
       </c>
@@ -2319,7 +2421,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:6">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B7" s="6" t="s">
         <v>0</v>
       </c>
@@ -2333,11 +2435,11 @@
         <v>39</v>
       </c>
     </row>
-    <row r="8" spans="1:6">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B8" s="6"/>
       <c r="C8" s="6"/>
     </row>
-    <row r="9" spans="1:6">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B9" s="6">
         <v>0</v>
       </c>
@@ -2357,7 +2459,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:6">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B10" s="6">
         <f>B9+$C$5</f>
         <v>0.25</v>
@@ -2378,7 +2480,7 @@
         <v>2.0833333333333332E-2</v>
       </c>
     </row>
-    <row r="11" spans="1:6">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B11" s="6">
         <f t="shared" ref="B11:B13" si="3">B10+$C$5</f>
         <v>0.5</v>
@@ -2399,7 +2501,7 @@
         <v>4.1666666666666664E-2</v>
       </c>
     </row>
-    <row r="12" spans="1:6">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B12" s="6">
         <f t="shared" si="3"/>
         <v>0.75</v>
@@ -2420,7 +2522,7 @@
         <v>0.1875</v>
       </c>
     </row>
-    <row r="13" spans="1:6">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B13" s="6">
         <f t="shared" si="3"/>
         <v>1</v>
@@ -2441,7 +2543,7 @@
         <v>8.3333333333333329E-2</v>
       </c>
     </row>
-    <row r="15" spans="1:6">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D15" t="s">
         <v>4</v>
       </c>
@@ -2454,7 +2556,7 @@
         <v>0.33333333333333331</v>
       </c>
     </row>
-    <row r="16" spans="1:6">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D16" t="s">
         <v>36</v>
       </c>
@@ -2465,7 +2567,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="17" spans="4:6">
+    <row r="17" spans="4:6" x14ac:dyDescent="0.25">
       <c r="D17" t="s">
         <v>18</v>
       </c>
@@ -2476,7 +2578,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="18" spans="4:6">
+    <row r="18" spans="4:6" x14ac:dyDescent="0.25">
       <c r="D18" t="s">
         <v>5</v>
       </c>
@@ -2487,18 +2589,18 @@
         <v>5</v>
       </c>
     </row>
-    <row r="19" spans="4:6">
+    <row r="19" spans="4:6" x14ac:dyDescent="0.25">
       <c r="F19" s="7">
         <f>1/3</f>
         <v>0.33333333333333331</v>
       </c>
     </row>
-    <row r="20" spans="4:6">
+    <row r="20" spans="4:6" x14ac:dyDescent="0.25">
       <c r="F20" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="21" spans="4:6">
+    <row r="21" spans="4:6" x14ac:dyDescent="0.25">
       <c r="F21" t="s">
         <v>5</v>
       </c>
@@ -2515,20 +2617,20 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:L45"/>
   <sheetViews>
     <sheetView zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
       <selection activeCell="F24" sqref="F24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="9.1640625" customWidth="1"/>
-    <col min="6" max="6" width="15.33203125" customWidth="1"/>
+    <col min="2" max="2" width="9.125" customWidth="1"/>
+    <col min="6" max="6" width="15.375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>37</v>
       </c>
@@ -2539,7 +2641,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:6">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>38</v>
       </c>
@@ -2550,7 +2652,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:6">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B3" s="1" t="s">
         <v>1</v>
       </c>
@@ -2561,7 +2663,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:6">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
         <v>2</v>
       </c>
@@ -2577,7 +2679,7 @@
         <v>0.16666666666666666</v>
       </c>
     </row>
-    <row r="6" spans="1:6">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="E6" t="s">
         <v>5</v>
       </c>
@@ -2585,7 +2687,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:6">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
         <v>0</v>
       </c>
@@ -2593,7 +2695,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="8" spans="1:6">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D8" t="s">
         <v>41</v>
       </c>
@@ -2601,7 +2703,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="9" spans="1:6">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B9">
         <v>1</v>
       </c>
@@ -2621,7 +2723,7 @@
         <v>0.16666666666666666</v>
       </c>
     </row>
-    <row r="10" spans="1:6">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B10">
         <f>B9+$C$5</f>
         <v>1.5</v>
@@ -2642,7 +2744,7 @@
         <v>0.44444444444444442</v>
       </c>
     </row>
-    <row r="11" spans="1:6">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B11">
         <f t="shared" ref="B11:B15" si="3">B10+$C$5</f>
         <v>2</v>
@@ -2663,7 +2765,7 @@
         <v>0.16666666666666666</v>
       </c>
     </row>
-    <row r="12" spans="1:6">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B12">
         <f t="shared" si="3"/>
         <v>2.5</v>
@@ -2684,7 +2786,7 @@
         <v>0.26666666666666666</v>
       </c>
     </row>
-    <row r="13" spans="1:6">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B13">
         <f t="shared" si="3"/>
         <v>3</v>
@@ -2705,7 +2807,7 @@
         <v>0.1111111111111111</v>
       </c>
     </row>
-    <row r="14" spans="1:6">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B14">
         <f t="shared" si="3"/>
         <v>3.5</v>
@@ -2726,7 +2828,7 @@
         <v>0.19047619047619047</v>
       </c>
     </row>
-    <row r="15" spans="1:6">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B15">
         <f t="shared" si="3"/>
         <v>4</v>
@@ -2747,12 +2849,12 @@
         <v>4.1666666666666664E-2</v>
       </c>
     </row>
-    <row r="16" spans="1:6">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="F16" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="17" spans="1:12">
+    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
       <c r="D17" t="s">
         <v>4</v>
       </c>
@@ -2765,7 +2867,7 @@
         <v>1.3876984126984127</v>
       </c>
     </row>
-    <row r="18" spans="1:12">
+    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
       <c r="D18" t="s">
         <v>34</v>
       </c>
@@ -2773,7 +2875,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="19" spans="1:12">
+    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
       <c r="C19" t="s">
         <v>33</v>
       </c>
@@ -2781,7 +2883,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="20" spans="1:12">
+    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
       <c r="D20">
         <v>4</v>
       </c>
@@ -2799,7 +2901,7 @@
       </c>
       <c r="L20" s="6"/>
     </row>
-    <row r="21" spans="1:12">
+    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
       <c r="H21" s="6">
         <v>1</v>
       </c>
@@ -2816,7 +2918,7 @@
         <v>1.2899137899138324E-3</v>
       </c>
     </row>
-    <row r="22" spans="1:12">
+    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
       <c r="F22" t="s">
         <v>5</v>
       </c>
@@ -2831,7 +2933,7 @@
       <c r="K22" s="6"/>
       <c r="L22" s="6"/>
     </row>
-    <row r="23" spans="1:12">
+    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B23" t="s">
         <v>13</v>
       </c>
@@ -2842,7 +2944,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="24" spans="1:12">
+    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B24" s="1" t="s">
         <v>14</v>
       </c>
@@ -2850,7 +2952,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="25" spans="1:12">
+    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B25" s="1" t="s">
         <v>1</v>
       </c>
@@ -2861,7 +2963,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="27" spans="1:12">
+    <row r="27" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B27" t="s">
         <v>2</v>
       </c>
@@ -2877,7 +2979,7 @@
         <v>8.3333333333333329E-2</v>
       </c>
     </row>
-    <row r="28" spans="1:12">
+    <row r="28" spans="1:12" x14ac:dyDescent="0.25">
       <c r="E28" t="s">
         <v>5</v>
       </c>
@@ -2885,7 +2987,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="29" spans="1:12">
+    <row r="29" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B29" t="s">
         <v>0</v>
       </c>
@@ -2893,7 +2995,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="31" spans="1:12">
+    <row r="31" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>43</v>
       </c>
@@ -2916,7 +3018,7 @@
         <v>8.3333333333333329E-2</v>
       </c>
     </row>
-    <row r="32" spans="1:12">
+    <row r="32" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>1</v>
       </c>
@@ -2940,7 +3042,7 @@
         <v>0.26666666666666666</v>
       </c>
     </row>
-    <row r="33" spans="1:6">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A33">
         <f>A32+1</f>
         <v>2</v>
@@ -2965,7 +3067,7 @@
         <v>0.1111111111111111</v>
       </c>
     </row>
-    <row r="34" spans="1:6">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A34">
         <f t="shared" ref="A34:A43" si="8">A33+1</f>
         <v>3</v>
@@ -2990,7 +3092,7 @@
         <v>0.19047619047619047</v>
       </c>
     </row>
-    <row r="35" spans="1:6">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A35">
         <f t="shared" si="8"/>
         <v>4</v>
@@ -3015,7 +3117,7 @@
         <v>8.3333333333333329E-2</v>
       </c>
     </row>
-    <row r="36" spans="1:6">
+    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A36">
         <f t="shared" si="8"/>
         <v>5</v>
@@ -3040,7 +3142,7 @@
         <v>0.14814814814814814</v>
       </c>
     </row>
-    <row r="37" spans="1:6">
+    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A37">
         <f t="shared" si="8"/>
         <v>6</v>
@@ -3065,7 +3167,7 @@
         <v>6.6666666666666666E-2</v>
       </c>
     </row>
-    <row r="38" spans="1:6">
+    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A38">
         <f t="shared" si="8"/>
         <v>7</v>
@@ -3090,7 +3192,7 @@
         <v>0.12121212121212122</v>
       </c>
     </row>
-    <row r="39" spans="1:6">
+    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A39">
         <f t="shared" si="8"/>
         <v>8</v>
@@ -3115,7 +3217,7 @@
         <v>5.5555555555555552E-2</v>
       </c>
     </row>
-    <row r="40" spans="1:6">
+    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A40">
         <f t="shared" si="8"/>
         <v>9</v>
@@ -3140,7 +3242,7 @@
         <v>0.10256410256410256</v>
       </c>
     </row>
-    <row r="41" spans="1:6">
+    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A41">
         <f t="shared" si="8"/>
         <v>10</v>
@@ -3165,7 +3267,7 @@
         <v>4.7619047619047616E-2</v>
       </c>
     </row>
-    <row r="42" spans="1:6">
+    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A42">
         <f t="shared" si="8"/>
         <v>11</v>
@@ -3190,7 +3292,7 @@
         <v>8.8888888888888878E-2</v>
       </c>
     </row>
-    <row r="43" spans="1:6">
+    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A43">
         <f t="shared" si="8"/>
         <v>12</v>
@@ -3215,12 +3317,12 @@
         <v>2.0833333333333332E-2</v>
       </c>
     </row>
-    <row r="44" spans="1:6">
+    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
       <c r="F44" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="45" spans="1:6">
+    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D45" t="s">
         <v>4</v>
       </c>
@@ -3245,24 +3347,24 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:I58"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A48" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="F21" sqref="F21"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="74" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
+      <selection activeCell="I25" sqref="I25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="9.1640625" customWidth="1"/>
+    <col min="2" max="2" width="9.125" customWidth="1"/>
     <col min="4" max="4" width="8.5" customWidth="1"/>
     <col min="5" max="5" width="18.5" customWidth="1"/>
-    <col min="6" max="6" width="16.6640625" customWidth="1"/>
-    <col min="8" max="8" width="23.83203125" customWidth="1"/>
-    <col min="9" max="9" width="19.83203125" customWidth="1"/>
+    <col min="6" max="6" width="16.625" customWidth="1"/>
+    <col min="8" max="8" width="23.875" customWidth="1"/>
+    <col min="9" max="9" width="19.875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>37</v>
       </c>
@@ -3273,7 +3375,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:8">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>38</v>
       </c>
@@ -3287,7 +3389,7 @@
       <c r="E2" s="1"/>
       <c r="F2" s="1"/>
     </row>
-    <row r="3" spans="1:8">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B3" s="12" t="s">
         <v>1</v>
       </c>
@@ -3298,7 +3400,7 @@
       <c r="E3" s="1"/>
       <c r="F3" s="1"/>
     </row>
-    <row r="4" spans="1:8">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B4" s="12" t="s">
         <v>6</v>
       </c>
@@ -3306,7 +3408,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="5" spans="1:8">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
         <v>2</v>
       </c>
@@ -3322,13 +3424,13 @@
         <v>3.6666666666666667E-2</v>
       </c>
     </row>
-    <row r="6" spans="1:8">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="D6">
         <f>EXP(GAMMALN(5))</f>
         <v>24.000000000000004</v>
       </c>
     </row>
-    <row r="7" spans="1:8">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
         <v>0</v>
       </c>
@@ -3336,7 +3438,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="8" spans="1:8">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C8" s="2" t="s">
         <v>9</v>
       </c>
@@ -3356,7 +3458,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="9" spans="1:8">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>0</v>
       </c>
@@ -3387,7 +3489,7 @@
         <v>1.422794665862785E-2</v>
       </c>
     </row>
-    <row r="10" spans="1:8">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10">
         <f>A9+1</f>
         <v>1</v>
@@ -3420,7 +3522,7 @@
         <v>5.6530751177242031E-2</v>
       </c>
     </row>
-    <row r="11" spans="1:8">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11">
         <f t="shared" ref="A11:A19" si="5">A10+1</f>
         <v>2</v>
@@ -3453,7 +3555,7 @@
         <v>2.7702937091885965E-2</v>
       </c>
     </row>
-    <row r="12" spans="1:8">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12">
         <f t="shared" si="5"/>
         <v>3</v>
@@ -3486,7 +3588,7 @@
         <v>5.3590165142477122E-2</v>
       </c>
     </row>
-    <row r="13" spans="1:8">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13">
         <f t="shared" si="5"/>
         <v>4</v>
@@ -3519,7 +3621,7 @@
         <v>2.5583310959814486E-2</v>
       </c>
     </row>
-    <row r="14" spans="1:8">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14">
         <f t="shared" si="5"/>
         <v>5</v>
@@ -3552,7 +3654,7 @@
         <v>4.824100794798538E-2</v>
       </c>
     </row>
-    <row r="15" spans="1:8">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15">
         <f t="shared" si="5"/>
         <v>6</v>
@@ -3585,7 +3687,7 @@
         <v>2.2466590145582454E-2</v>
       </c>
     </row>
-    <row r="16" spans="1:8">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16">
         <f t="shared" si="5"/>
         <v>7</v>
@@ -3618,7 +3720,7 @@
         <v>4.1368062472973033E-2</v>
       </c>
     </row>
-    <row r="17" spans="1:9">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17">
         <f t="shared" si="5"/>
         <v>8</v>
@@ -3651,7 +3753,7 @@
         <v>1.8833638590747683E-2</v>
       </c>
     </row>
-    <row r="18" spans="1:9">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18">
         <f t="shared" si="5"/>
         <v>9</v>
@@ -3661,7 +3763,7 @@
         <v>0.99</v>
       </c>
       <c r="C18" s="2">
-        <f t="shared" ref="C10:C19" si="7">1+(B18^2/$C$4)</f>
+        <f t="shared" ref="C18:C19" si="7">1+(B18^2/$C$4)</f>
         <v>1.1089</v>
       </c>
       <c r="D18" s="2">
@@ -3684,13 +3786,13 @@
         <v>3.3942224550243344E-2</v>
       </c>
     </row>
-    <row r="19" spans="1:9">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19">
         <f t="shared" si="5"/>
         <v>10</v>
       </c>
       <c r="B19" s="12">
-        <f t="shared" ref="B11:B19" si="8">B18+$C$5</f>
+        <f t="shared" ref="B19" si="8">B18+$C$5</f>
         <v>1.1000000000000001</v>
       </c>
       <c r="C19" s="2">
@@ -3717,7 +3819,7 @@
         <v>7.5722695489778688E-3</v>
       </c>
     </row>
-    <row r="21" spans="1:9">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="C21" s="5">
         <f>SUM(C9:C19)</f>
         <v>11.517611111111112</v>
@@ -3734,7 +3836,7 @@
         <v>0.35005890428655723</v>
       </c>
     </row>
-    <row r="22" spans="1:9">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="G22" t="s">
         <v>5</v>
       </c>
@@ -3742,7 +3844,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="24" spans="1:9">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="G24" t="s">
         <v>22</v>
       </c>
@@ -3750,7 +3852,7 @@
         <v>1.0000000000000001E-5</v>
       </c>
     </row>
-    <row r="25" spans="1:9">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
       <c r="G25" t="s">
         <v>24</v>
       </c>
@@ -3763,7 +3865,7 @@
         <v>7.4038856179998169E-3</v>
       </c>
     </row>
-    <row r="26" spans="1:9">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
       <c r="G26" t="s">
         <v>25</v>
       </c>
@@ -3772,12 +3874,12 @@
         <v>0.35746278990455704</v>
       </c>
     </row>
-    <row r="27" spans="1:9">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
       <c r="H27" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="28" spans="1:9">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B28" t="s">
         <v>13</v>
       </c>
@@ -3785,7 +3887,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:9">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B29" s="1" t="s">
         <v>0</v>
       </c>
@@ -3796,7 +3898,7 @@
       <c r="E29" s="1"/>
       <c r="F29" s="1"/>
     </row>
-    <row r="30" spans="1:9">
+    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B30" s="1" t="s">
         <v>1</v>
       </c>
@@ -3807,7 +3909,7 @@
       <c r="E30" s="1"/>
       <c r="F30" s="1"/>
     </row>
-    <row r="31" spans="1:9">
+    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B31" t="s">
         <v>6</v>
       </c>
@@ -3815,7 +3917,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="32" spans="1:9">
+    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B32" t="s">
         <v>2</v>
       </c>
@@ -3831,13 +3933,13 @@
         <v>1.8333333333333333E-2</v>
       </c>
     </row>
-    <row r="33" spans="1:8">
+    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
       <c r="D33">
         <f>EXP(GAMMALN(5))</f>
         <v>24.000000000000004</v>
       </c>
     </row>
-    <row r="34" spans="1:8">
+    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B34" t="s">
         <v>0</v>
       </c>
@@ -3845,7 +3947,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="35" spans="1:8">
+    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C35" s="2" t="s">
         <v>9</v>
       </c>
@@ -3859,7 +3961,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="36" spans="1:8">
+    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>0</v>
       </c>
@@ -3890,7 +3992,7 @@
         <v>7.2183798003644098E-3</v>
       </c>
     </row>
-    <row r="37" spans="1:8">
+    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A37">
         <f>A36+1</f>
         <v>1</v>
@@ -3923,7 +4025,7 @@
         <v>2.8827589747663977E-2</v>
       </c>
     </row>
-    <row r="38" spans="1:8">
+    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A38">
         <f t="shared" ref="A38:A56" si="14">A37+1</f>
         <v>2</v>
@@ -3956,7 +4058,7 @@
         <v>1.4345141448041158E-2</v>
       </c>
     </row>
-    <row r="39" spans="1:8">
+    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A39">
         <f t="shared" si="14"/>
         <v>3</v>
@@ -3989,7 +4091,7 @@
         <v>2.8463034013958683E-2</v>
       </c>
     </row>
-    <row r="40" spans="1:8">
+    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A40">
         <f t="shared" si="14"/>
         <v>4</v>
@@ -4022,7 +4124,7 @@
         <v>1.407410255169796E-2</v>
       </c>
     </row>
-    <row r="41" spans="1:8">
+    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A41">
         <f t="shared" si="14"/>
         <v>5</v>
@@ -4055,7 +4157,7 @@
         <v>2.7749040299430223E-2</v>
       </c>
     </row>
-    <row r="42" spans="1:8">
+    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A42">
         <f t="shared" si="14"/>
         <v>6</v>
@@ -4088,7 +4190,7 @@
         <v>1.3634802678083213E-2</v>
       </c>
     </row>
-    <row r="43" spans="1:8">
+    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A43">
         <f t="shared" si="14"/>
         <v>7</v>
@@ -4121,7 +4223,7 @@
         <v>2.6714712824863589E-2</v>
       </c>
     </row>
-    <row r="44" spans="1:8">
+    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A44">
         <f t="shared" si="14"/>
         <v>8</v>
@@ -4154,7 +4256,7 @@
         <v>1.304491749913235E-2</v>
       </c>
     </row>
-    <row r="45" spans="1:8">
+    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A45">
         <f t="shared" si="14"/>
         <v>9</v>
@@ -4187,7 +4289,7 @@
         <v>2.5401006986823373E-2</v>
       </c>
     </row>
-    <row r="46" spans="1:8">
+    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A46">
         <f t="shared" si="14"/>
         <v>10</v>
@@ -4220,7 +4322,7 @@
         <v>1.2327361247871267E-2</v>
       </c>
     </row>
-    <row r="47" spans="1:8">
+    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A47">
         <f t="shared" si="14"/>
         <v>11</v>
@@ -4253,7 +4355,7 @@
         <v>2.3857824982118161E-2</v>
       </c>
     </row>
-    <row r="48" spans="1:8">
+    <row r="48" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A48">
         <f t="shared" si="14"/>
         <v>12</v>
@@ -4286,7 +4388,7 @@
         <v>1.1508698444248427E-2</v>
       </c>
     </row>
-    <row r="49" spans="1:8">
+    <row r="49" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A49">
         <f t="shared" si="14"/>
         <v>13</v>
@@ -4319,7 +4421,7 @@
         <v>2.2140649576504069E-2</v>
       </c>
     </row>
-    <row r="50" spans="1:8">
+    <row r="50" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A50">
         <f t="shared" si="14"/>
         <v>14</v>
@@ -4352,7 +4454,7 @@
         <v>1.061740821465639E-2</v>
       </c>
     </row>
-    <row r="51" spans="1:8">
+    <row r="51" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A51">
         <f t="shared" si="14"/>
         <v>15</v>
@@ -4385,7 +4487,7 @@
         <v>2.0307051365225551E-2</v>
       </c>
     </row>
-    <row r="52" spans="1:8">
+    <row r="52" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A52">
         <f t="shared" si="14"/>
         <v>16</v>
@@ -4418,7 +4520,7 @@
         <v>9.6821673597944549E-3</v>
       </c>
     </row>
-    <row r="53" spans="1:8">
+    <row r="53" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A53">
         <f t="shared" si="14"/>
         <v>17</v>
@@ -4451,7 +4553,7 @@
         <v>1.8413388123349972E-2</v>
       </c>
     </row>
-    <row r="54" spans="1:8">
+    <row r="54" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A54">
         <f t="shared" si="14"/>
         <v>18</v>
@@ -4484,7 +4586,7 @@
         <v>8.7302998246421171E-3</v>
       </c>
     </row>
-    <row r="55" spans="1:8">
+    <row r="55" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A55">
         <f t="shared" si="14"/>
         <v>19</v>
@@ -4517,7 +4619,7 @@
         <v>1.6511960126742678E-2</v>
       </c>
     </row>
-    <row r="56" spans="1:8">
+    <row r="56" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A56">
         <f t="shared" si="14"/>
         <v>20</v>
@@ -4550,7 +4652,7 @@
         <v>3.8932527893450375E-3</v>
       </c>
     </row>
-    <row r="58" spans="1:8">
+    <row r="58" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C58" s="5">
         <f>SUM(C36:C56)</f>
         <v>21.456934210526313</v>

</xml_diff>